<commit_message>
Todo impreso y adaptado
</commit_message>
<xml_diff>
--- a/Recetatic/REcetario.xlsx
+++ b/Recetatic/REcetario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Worome\source\repos\Recetatic\Recetatic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Script\source\repos\Recetatic\Recetatic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D767F05B-2077-4C96-9F28-39250C191EED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02D218B-7E1D-4C83-89CD-845B9BEA83B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{7CEDE6BF-7572-4931-BC0D-5229394BEFD2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" firstSheet="3" activeTab="7" xr2:uid="{7CEDE6BF-7572-4931-BC0D-5229394BEFD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionalidades" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="Autores" sheetId="6" r:id="rId4"/>
     <sheet name="Menús semanales y eventos" sheetId="4" r:id="rId5"/>
     <sheet name="Histórico de recetas" sheetId="3" r:id="rId6"/>
-    <sheet name="Recetas" sheetId="1" r:id="rId7"/>
+    <sheet name="Recetas Express" sheetId="1" r:id="rId7"/>
+    <sheet name="Recetas Completas" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -463,7 +464,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,8 +487,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="24">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -626,6 +634,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -691,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -709,99 +729,106 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1118,263 +1145,263 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A57034A-7242-4292-96B6-8B73EA316F50}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.140625" customWidth="1"/>
+    <col min="1" max="1" width="45.88671875" customWidth="1"/>
+    <col min="2" max="2" width="40.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="56" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="57" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+    <row r="11" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="56"/>
+      <c r="B11" s="58" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="55" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="54"/>
+      <c r="B18" s="55" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="54"/>
+      <c r="B19" s="55" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="54"/>
+      <c r="B20" s="55" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="54"/>
+      <c r="B21" s="55" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="54"/>
+      <c r="B22" s="55" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="54"/>
+      <c r="B23" s="55" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="54"/>
+      <c r="B24" s="55" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="54"/>
+      <c r="B25" s="55" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="54"/>
+      <c r="B26" s="55" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>126</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A17:A26"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10BCEE83-0BFF-4296-922C-52DFDD52A48D}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>132</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="31"/>
+      <c r="B4" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="31"/>
+      <c r="B5" s="11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="31"/>
+      <c r="B6" s="11" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>138</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>139</v>
       </c>
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>140</v>
       </c>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>128</v>
       </c>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>141</v>
       </c>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>60</v>
       </c>
@@ -1397,128 +1424,128 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>106</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="32"/>
+      <c r="B5" s="12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="32"/>
+      <c r="B6" s="12" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>112</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>113</v>
       </c>
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>115</v>
       </c>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>116</v>
       </c>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>117</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>119</v>
       </c>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>120</v>
       </c>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>121</v>
       </c>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>122</v>
       </c>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>123</v>
       </c>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>124</v>
       </c>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>125</v>
       </c>
@@ -1529,6 +1556,7 @@
     <mergeCell ref="A4:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1540,45 +1568,46 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>131</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1590,85 +1619,85 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>99</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>100</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="20"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="17" t="s">
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="34"/>
+      <c r="B5" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="34"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="34"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="34"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="34"/>
+      <c r="B9" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="20"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20" t="s">
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="34"/>
+      <c r="B10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1676,6 +1705,7 @@
     <mergeCell ref="A4:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1687,52 +1717,52 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>91</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>92</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="22" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="35"/>
+      <c r="B5" s="15" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="35"/>
+      <c r="B6" s="15" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="35"/>
+      <c r="B7" s="15" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1741,687 +1771,748 @@
     <mergeCell ref="A4:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB3D7B3-CE46-4308-91D2-98C2D11AC8E9}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="24" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="49"/>
+      <c r="B5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
-      <c r="B6" s="24" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="49"/>
+      <c r="B6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="24" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="49"/>
+      <c r="B7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
-      <c r="B8" s="24" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="49"/>
+      <c r="B8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="49"/>
+      <c r="B9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="6"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="6"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="25" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="29"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="50"/>
+      <c r="B18" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="29"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="26" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="18"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>131</v>
       </c>
       <c r="B20" s="6"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D21" s="29"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D22" s="29"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D23" s="29"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D24" s="29"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D25" s="29"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D26" s="29"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D27" s="29"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D28" s="29"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="G28" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D29" s="29"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D30" s="29"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D31" s="29"/>
-      <c r="E31" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="F31" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D32" s="29"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D33" s="29"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D34" s="29"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D35" s="29"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="G35" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="H35" s="5"/>
-    </row>
-    <row r="36" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D36" s="29"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="H36" s="5"/>
-    </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D37" s="29"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="51" t="s">
-        <v>69</v>
-      </c>
-      <c r="H37" s="52" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D38" s="29"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="51"/>
-      <c r="H38" s="52" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D39" s="29"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="51"/>
-      <c r="H39" s="52" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D40" s="29"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="50" t="s">
-        <v>72</v>
-      </c>
-      <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D41" s="29"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D42" s="29"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D43" s="29"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D44" s="29"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-    </row>
-    <row r="45" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D45" s="29"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-    </row>
-    <row r="46" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D46" s="29"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-    </row>
-    <row r="47" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D47" s="29"/>
-      <c r="E47" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="F47" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-    </row>
-    <row r="48" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D48" s="29"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D49" s="29"/>
-      <c r="E49" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="F49" s="53" t="s">
-        <v>15</v>
-      </c>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D50" s="29"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-    </row>
-    <row r="51" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D51" s="29"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-    </row>
-    <row r="52" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D52" s="29"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-    </row>
-    <row r="53" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D53" s="29"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-    </row>
-    <row r="54" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="29"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-    </row>
-    <row r="55" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="29"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-    </row>
-    <row r="56" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D56" s="29"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="54" t="s">
-        <v>64</v>
-      </c>
-      <c r="G56" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="H56" s="5"/>
-    </row>
-    <row r="57" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D57" s="29"/>
-      <c r="E57" s="34"/>
-      <c r="F57" s="54"/>
-      <c r="G57" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="H57" s="5"/>
-    </row>
-    <row r="58" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D58" s="29"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-    </row>
-    <row r="59" spans="4:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D59" s="30"/>
-      <c r="E59" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="G37:G39"/>
-    <mergeCell ref="F35:F42"/>
-    <mergeCell ref="E31:E46"/>
-    <mergeCell ref="E49:E58"/>
-    <mergeCell ref="D8:D59"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="E8:E30"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="F20:F23"/>
+  <mergeCells count="2">
     <mergeCell ref="A4:A9"/>
     <mergeCell ref="A17:A18"/>
-    <mergeCell ref="F8:F13"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="F18:F19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D51528C-81F5-41FE-ABAF-16607AA15D0F}">
+  <dimension ref="A1:E59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="41"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="41"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="41"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A12" s="41"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="41"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="41"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="41"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="41"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="41"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A18" s="41"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A19" s="41"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="41"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A21" s="41"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A22" s="41"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="41"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A24" s="41"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A25" s="41"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A26" s="41"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A27" s="41"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A28" s="41"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A29" s="41"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A30" s="41"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A31" s="41"/>
+      <c r="B31" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A32" s="41"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A33" s="41"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A34" s="41"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A35" s="41"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A36" s="41"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="41"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="41"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="41"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A40" s="41"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A41" s="41"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A42" s="41"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A43" s="41"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A44" s="41"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A45" s="41"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A46" s="41"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A47" s="41"/>
+      <c r="B47" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+    </row>
+    <row r="48" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A48" s="41"/>
+      <c r="B48" s="46"/>
+      <c r="C48" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A49" s="41"/>
+      <c r="B49" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+    </row>
+    <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A50" s="41"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+    </row>
+    <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A51" s="41"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A52" s="41"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+    </row>
+    <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A53" s="41"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+    </row>
+    <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A54" s="41"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+    </row>
+    <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A55" s="41"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+    </row>
+    <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A56" s="41"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56" s="5"/>
+    </row>
+    <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A57" s="41"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="5"/>
+    </row>
+    <row r="58" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A58" s="41"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+    </row>
+    <row r="59" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A59" s="42"/>
+      <c r="B59" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B49:B58"/>
+    <mergeCell ref="A8:A59"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="B8:B30"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="C35:C42"/>
+    <mergeCell ref="B31:B46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Inserción y consulta de datos
</commit_message>
<xml_diff>
--- a/Recetatic/REcetario.xlsx
+++ b/Recetatic/REcetario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Script\source\repos\Recetatic\Recetatic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Worome\source\repos\Recetatic\Recetatic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403B2D93-A3D5-4824-8A67-2803C2F9CFEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B270876-983A-4D82-BB4A-DE2551DEBD65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="1" xr2:uid="{7CEDE6BF-7572-4931-BC0D-5229394BEFD2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{7CEDE6BF-7572-4931-BC0D-5229394BEFD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionalidades" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="159">
   <si>
     <t>EXPRESS</t>
   </si>
@@ -300,9 +300,6 @@
   </si>
   <si>
     <t>Fecha de incorporación</t>
-  </si>
-  <si>
-    <t>En la rejilla de rectas, poner un buscador en el que se pueda buscar por alguno de estos campos ( en los campos que son string debe buscarse por una parte de la cadena):</t>
   </si>
   <si>
     <t>Fecha</t>
@@ -511,12 +508,59 @@
   <si>
     <t>URL de otras recomandaciones para obtener iconos: https://esferacreativa.com/crear-iconos-online-herramientas/</t>
   </si>
+  <si>
+    <t>En la rejilla de recetas, poner un buscador en el que se pueda buscar por alguno de estos campos ( en los campos que son string debe buscarse por una parte de la cadena):</t>
+  </si>
+  <si>
+    <t>AcceptButton</t>
+  </si>
+  <si>
+    <t>CancelButton</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Al crear una tabla en el panel de las propiedades, existe el apartado </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Especificación de identidad </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>para cada campo, en el que se puede especificar si es autoincrementable en la propiedad (Es una entidad).</t>
+    </r>
+  </si>
+  <si>
+    <t>TabIndex</t>
+  </si>
+  <si>
+    <t>TabStop</t>
+  </si>
+  <si>
+    <t>MaxLength</t>
+  </si>
+  <si>
+    <t>CharacterCasing</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -558,6 +602,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="27">
@@ -826,6 +878,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -903,9 +958,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1223,151 +1275,151 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A57034A-7242-4292-96B6-8B73EA316F50}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.88671875" customWidth="1"/>
-    <col min="2" max="2" width="40.109375" customWidth="1"/>
+    <col min="1" max="1" width="45.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="36" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
         <v>80</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="37"/>
       <c r="B11" s="33" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
-        <v>89</v>
+    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>151</v>
       </c>
       <c r="B17" s="31" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="35"/>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
       <c r="B18" s="31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="36"/>
       <c r="B19" s="31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
       <c r="B20" s="31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="36"/>
       <c r="B21" s="31" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="36"/>
       <c r="B22" s="31" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="36"/>
       <c r="B23" s="31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="36"/>
       <c r="B24" s="31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="36"/>
       <c r="B25" s="31" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="36"/>
       <c r="B26" s="31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1382,74 +1434,115 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACFA3BB-9883-40C7-BCA9-F4350A092249}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="34" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+      <c r="B2" s="34" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="37"/>
-      <c r="B2" s="34" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="38"/>
+      <c r="B3" s="34" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="37"/>
-      <c r="B3" s="34" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="38"/>
+      <c r="B4" s="34" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
-      <c r="B4" s="34" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="38"/>
+      <c r="B5" s="34" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
-      <c r="B5" s="34" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="38"/>
+      <c r="B6" s="34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
+      <c r="B7" s="34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="38"/>
+      <c r="B8" s="34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
+      <c r="B9" s="34" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="38"/>
+      <c r="B11" s="34" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
+      <c r="B12" s="34" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
-      <c r="B6" s="34" t="s">
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="61" t="s">
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+    <row r="17" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>151</v>
+    <row r="19" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="A1:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1464,98 +1557,98 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="11" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="39"/>
+      <c r="B4" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
-      <c r="B4" s="11" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="39"/>
+      <c r="B5" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="11" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="38"/>
-      <c r="B6" s="11" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B10" s="6"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B11" s="6"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="6"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B13" s="6"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>60</v>
       </c>
@@ -1578,130 +1671,130 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="12" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="40"/>
+      <c r="B5" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
-      <c r="B5" s="12" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="40"/>
+      <c r="B6" s="12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="39"/>
-      <c r="B6" s="12" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="6"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="6"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B12" s="6"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="6"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B14" s="6"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B15" s="6"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="B20" s="6"/>
     </row>
@@ -1722,41 +1815,41 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1773,81 +1866,81 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="42"/>
+      <c r="B5" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="14"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
-      <c r="B5" s="40" t="s">
+      <c r="C5" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="42"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="42"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="42"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="42"/>
+      <c r="B9" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="41"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="41"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="41"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="41"/>
-      <c r="B9" s="14" t="s">
-        <v>104</v>
-      </c>
       <c r="C9" s="14"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="42"/>
       <c r="B10" s="14" t="s">
         <v>11</v>
       </c>
@@ -1871,53 +1964,53 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="6"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
+      <c r="B4" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="15" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="43"/>
+      <c r="B5" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="42"/>
-      <c r="B5" s="15" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="43"/>
+      <c r="B6" s="15" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="42"/>
-      <c r="B6" s="15" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="43"/>
+      <c r="B7" s="15" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="42"/>
-      <c r="B7" s="15" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1937,134 +2030,134 @@
       <selection activeCell="D1" sqref="D1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="43" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="43"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="44"/>
       <c r="B5" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="43"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="44"/>
       <c r="B6" s="16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="43"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="44"/>
       <c r="B7" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="43"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="44"/>
       <c r="B8" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="43"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="44"/>
       <c r="B9" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="44" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="45" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="44"/>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="45"/>
       <c r="B18" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="18"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B20" s="6"/>
     </row>
@@ -2086,14 +2179,14 @@
       <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2101,7 +2194,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -2110,7 +2203,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2119,7 +2212,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>55</v>
       </c>
@@ -2128,7 +2221,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -2137,7 +2230,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -2146,23 +2239,23 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="49" t="s">
+    <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="59" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="20" t="s">
@@ -2170,55 +2263,55 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="50"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="58"/>
+    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="51"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="59"/>
       <c r="D9" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="58"/>
+    <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="20" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="50"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="58"/>
+    <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="51"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="50"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="58"/>
+    <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="51"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="59"/>
       <c r="D12" s="20" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="50"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="58"/>
+    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="51"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="59"/>
       <c r="D13" s="20" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="50"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="59" t="s">
+    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="60" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="21" t="s">
@@ -2226,37 +2319,37 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="50"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="59"/>
+    <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="51"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="60"/>
       <c r="D15" s="21" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="50"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="59"/>
+    <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="51"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="60"/>
       <c r="D16" s="21" t="s">
         <v>34</v>
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="50"/>
-      <c r="B17" s="54"/>
-      <c r="C17" s="59"/>
+    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="51"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="60"/>
       <c r="D17" s="21" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="50"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="60" t="s">
+    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="51"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="61" t="s">
         <v>35</v>
       </c>
       <c r="D18" s="22" t="s">
@@ -2264,19 +2357,19 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="50"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="60"/>
+    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="51"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="22" t="s">
         <v>37</v>
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="50"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="57" t="s">
+    <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="51"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="58" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="23" t="s">
@@ -2284,37 +2377,37 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A21" s="50"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="57"/>
+    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="51"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="58"/>
       <c r="D21" s="23" t="s">
         <v>40</v>
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A22" s="50"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="57"/>
+    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="51"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="58"/>
       <c r="D22" s="23" t="s">
         <v>41</v>
       </c>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="50"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="57"/>
+    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="51"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="58"/>
       <c r="D23" s="23" t="s">
         <v>42</v>
       </c>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A24" s="50"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="52" t="s">
+    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="51"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="53" t="s">
         <v>43</v>
       </c>
       <c r="D24" s="24" t="s">
@@ -2322,37 +2415,37 @@
       </c>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A25" s="50"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="52"/>
+    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="51"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="53"/>
       <c r="D25" s="24" t="s">
         <v>45</v>
       </c>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A26" s="50"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="52"/>
+    <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="51"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="53"/>
       <c r="D26" s="24" t="s">
         <v>46</v>
       </c>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A27" s="50"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="52"/>
+    <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="51"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="53"/>
       <c r="D27" s="24" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A28" s="50"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="53" t="s">
+    <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="51"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="54" t="s">
         <v>47</v>
       </c>
       <c r="D28" s="25" t="s">
@@ -2360,27 +2453,27 @@
       </c>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A29" s="50"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="53"/>
+    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="51"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="54"/>
       <c r="D29" s="25" t="s">
         <v>49</v>
       </c>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="50"/>
-      <c r="B30" s="54"/>
-      <c r="C30" s="53"/>
+    <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="51"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="54"/>
       <c r="D30" s="25" t="s">
         <v>50</v>
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A31" s="50"/>
-      <c r="B31" s="47" t="s">
+    <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="51"/>
+      <c r="B31" s="48" t="s">
         <v>51</v>
       </c>
       <c r="C31" s="26" t="s">
@@ -2389,37 +2482,37 @@
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A32" s="50"/>
-      <c r="B32" s="47"/>
+    <row r="32" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="51"/>
+      <c r="B32" s="48"/>
       <c r="C32" s="26" t="s">
         <v>52</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A33" s="50"/>
-      <c r="B33" s="47"/>
+    <row r="33" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="51"/>
+      <c r="B33" s="48"/>
       <c r="C33" s="26" t="s">
         <v>53</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A34" s="50"/>
-      <c r="B34" s="47"/>
+    <row r="34" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="51"/>
+      <c r="B34" s="48"/>
       <c r="C34" s="26" t="s">
         <v>54</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A35" s="50"/>
-      <c r="B35" s="47"/>
-      <c r="C35" s="46" t="s">
+    <row r="35" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="51"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="47" t="s">
         <v>66</v>
       </c>
       <c r="D35" s="27" t="s">
@@ -2427,110 +2520,110 @@
       </c>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A36" s="50"/>
-      <c r="B36" s="47"/>
-      <c r="C36" s="46"/>
+    <row r="36" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="51"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="47"/>
       <c r="D36" s="27" t="s">
         <v>68</v>
       </c>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="50"/>
-      <c r="B37" s="47"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="45" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="51"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="46" t="s">
         <v>69</v>
       </c>
       <c r="E37" s="28" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="50"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="46"/>
-      <c r="D38" s="45"/>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="51"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="46"/>
       <c r="E38" s="28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="50"/>
-      <c r="B39" s="47"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="45"/>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="51"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="46"/>
       <c r="E39" s="28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A40" s="50"/>
-      <c r="B40" s="47"/>
-      <c r="C40" s="46"/>
+    <row r="40" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="51"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="47"/>
       <c r="D40" s="27" t="s">
         <v>72</v>
       </c>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A41" s="50"/>
-      <c r="B41" s="47"/>
-      <c r="C41" s="46"/>
+    <row r="41" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="51"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="47"/>
       <c r="D41" s="27" t="s">
         <v>73</v>
       </c>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A42" s="50"/>
-      <c r="B42" s="47"/>
-      <c r="C42" s="46"/>
+    <row r="42" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="51"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="47"/>
       <c r="D42" s="27" t="s">
         <v>74</v>
       </c>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A43" s="50"/>
-      <c r="B43" s="47"/>
+    <row r="43" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="51"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="26" t="s">
         <v>75</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A44" s="50"/>
-      <c r="B44" s="47"/>
+    <row r="44" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="51"/>
+      <c r="B44" s="48"/>
       <c r="C44" s="26" t="s">
         <v>76</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A45" s="50"/>
-      <c r="B45" s="47"/>
+    <row r="45" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="51"/>
+      <c r="B45" s="48"/>
       <c r="C45" s="26" t="s">
         <v>77</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
     </row>
-    <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A46" s="50"/>
-      <c r="B46" s="47"/>
+    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="51"/>
+      <c r="B46" s="48"/>
       <c r="C46" s="26" t="s">
         <v>78</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
     </row>
-    <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A47" s="50"/>
-      <c r="B47" s="55" t="s">
+    <row r="47" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="51"/>
+      <c r="B47" s="56" t="s">
         <v>56</v>
       </c>
       <c r="C47" s="20" t="s">
@@ -2539,18 +2632,18 @@
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A48" s="50"/>
-      <c r="B48" s="55"/>
+    <row r="48" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="51"/>
+      <c r="B48" s="56"/>
       <c r="C48" s="20" t="s">
         <v>58</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A49" s="50"/>
-      <c r="B49" s="48" t="s">
+    <row r="49" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="51"/>
+      <c r="B49" s="49" t="s">
         <v>59</v>
       </c>
       <c r="C49" s="29" t="s">
@@ -2559,64 +2652,64 @@
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A50" s="50"/>
-      <c r="B50" s="48"/>
+    <row r="50" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="51"/>
+      <c r="B50" s="49"/>
       <c r="C50" s="29" t="s">
         <v>60</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A51" s="50"/>
-      <c r="B51" s="48"/>
+    <row r="51" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="51"/>
+      <c r="B51" s="49"/>
       <c r="C51" s="29" t="s">
         <v>61</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A52" s="50"/>
-      <c r="B52" s="48"/>
+    <row r="52" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="51"/>
+      <c r="B52" s="49"/>
       <c r="C52" s="29" t="s">
         <v>16</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
-    <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A53" s="50"/>
-      <c r="B53" s="48"/>
+    <row r="53" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="51"/>
+      <c r="B53" s="49"/>
       <c r="C53" s="29" t="s">
         <v>62</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A54" s="50"/>
-      <c r="B54" s="48"/>
+    <row r="54" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="51"/>
+      <c r="B54" s="49"/>
       <c r="C54" s="29" t="s">
         <v>63</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A55" s="50"/>
-      <c r="B55" s="48"/>
+    <row r="55" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="51"/>
+      <c r="B55" s="49"/>
       <c r="C55" s="29" t="s">
         <v>17</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
     </row>
-    <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A56" s="50"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="56" t="s">
+    <row r="56" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A56" s="51"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="57" t="s">
         <v>64</v>
       </c>
       <c r="D56" s="30" t="s">
@@ -2624,26 +2717,26 @@
       </c>
       <c r="E56" s="5"/>
     </row>
-    <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A57" s="50"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="56"/>
+    <row r="57" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="51"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="57"/>
       <c r="D57" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E57" s="5"/>
     </row>
-    <row r="58" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A58" s="50"/>
-      <c r="B58" s="48"/>
+    <row r="58" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="51"/>
+      <c r="B58" s="49"/>
       <c r="C58" s="29" t="s">
         <v>65</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
     </row>
-    <row r="59" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A59" s="51"/>
+    <row r="59" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="52"/>
       <c r="B59" s="19" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
Optimización formulario y tabla de perioricidad
</commit_message>
<xml_diff>
--- a/Recetatic/REcetario.xlsx
+++ b/Recetatic/REcetario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Worome\source\repos\Recetatic\Recetatic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Script\source\repos\Recetatic\Recetatic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B270876-983A-4D82-BB4A-DE2551DEBD65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4E587B-88EF-4AF8-9139-8A672A18ED11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{7CEDE6BF-7572-4931-BC0D-5229394BEFD2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="1" xr2:uid="{7CEDE6BF-7572-4931-BC0D-5229394BEFD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionalidades" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="159">
   <si>
     <t>EXPRESS</t>
   </si>
@@ -834,7 +834,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -959,6 +959,10 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1279,49 +1283,49 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" customWidth="1"/>
+    <col min="1" max="1" width="45.88671875" customWidth="1"/>
+    <col min="2" max="2" width="40.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
         <v>80</v>
       </c>
@@ -1329,23 +1333,23 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="37"/>
       <c r="B11" s="33" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="36" t="s">
         <v>151</v>
       </c>
@@ -1353,71 +1357,71 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="36"/>
       <c r="B18" s="31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="36"/>
       <c r="B19" s="31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="36"/>
       <c r="B20" s="31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="36"/>
       <c r="B21" s="31" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="36"/>
       <c r="B22" s="31" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="36"/>
       <c r="B23" s="31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="36"/>
       <c r="B24" s="31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="36"/>
       <c r="B25" s="31" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="36"/>
       <c r="B26" s="31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>125</v>
       </c>
@@ -1434,19 +1438,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACFA3BB-9883-40C7-BCA9-F4350A092249}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
         <v>141</v>
       </c>
@@ -1454,95 +1458,113 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="38"/>
       <c r="B2" s="34" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="38"/>
       <c r="B3" s="34" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="38"/>
       <c r="B4" s="34" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="38"/>
       <c r="B5" s="34" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="38"/>
       <c r="B6" s="34" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="38"/>
       <c r="B7" s="34" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="38"/>
       <c r="B8" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="62" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="63" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="62"/>
+      <c r="B11" s="63" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="62"/>
+      <c r="B12" s="63" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="34" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="62"/>
+      <c r="B13" s="63" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="34" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="62"/>
+      <c r="B14" s="63" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="34" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="62"/>
+      <c r="B15" s="63" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="34" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+    <row r="17" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="35" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+    <row r="19" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+    </row>
+    <row r="21" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+    <row r="23" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
         <v>154</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:A12"/>
+  <mergeCells count="2">
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A1:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1557,24 +1579,24 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
         <v>132</v>
       </c>
@@ -1582,73 +1604,73 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="39"/>
       <c r="B4" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="39"/>
       <c r="B5" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="39"/>
       <c r="B6" s="11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>137</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>138</v>
       </c>
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>139</v>
       </c>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>127</v>
       </c>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>128</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>140</v>
       </c>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>60</v>
       </c>
@@ -1671,30 +1693,30 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>105</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>106</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="40" t="s">
         <v>107</v>
       </c>
@@ -1702,97 +1724,97 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="40"/>
       <c r="B5" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="40"/>
       <c r="B6" s="12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>111</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>112</v>
       </c>
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>113</v>
       </c>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>115</v>
       </c>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>116</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>117</v>
       </c>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>119</v>
       </c>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>120</v>
       </c>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>121</v>
       </c>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>122</v>
       </c>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>123</v>
       </c>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>124</v>
       </c>
@@ -1815,39 +1837,39 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>130</v>
       </c>
@@ -1866,34 +1888,34 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>99</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>100</v>
       </c>
@@ -1902,7 +1924,7 @@
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="42"/>
       <c r="B5" s="41" t="s">
         <v>102</v>
@@ -1911,35 +1933,35 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="42"/>
       <c r="B6" s="41"/>
       <c r="C6" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="42"/>
       <c r="B7" s="41"/>
       <c r="C7" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="42"/>
       <c r="B8" s="41"/>
       <c r="C8" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="42"/>
       <c r="B9" s="14" t="s">
         <v>103</v>
       </c>
       <c r="C9" s="14"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="42"/>
       <c r="B10" s="14" t="s">
         <v>11</v>
@@ -1964,30 +1986,30 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>91</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="43" t="s">
         <v>92</v>
       </c>
@@ -1995,19 +2017,19 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="43"/>
       <c r="B5" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="43"/>
       <c r="B6" s="15" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="43"/>
       <c r="B7" s="15" t="s">
         <v>96</v>
@@ -2030,32 +2052,32 @@
       <selection activeCell="D1" sqref="D1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="44" t="s">
         <v>4</v>
       </c>
@@ -2063,79 +2085,79 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="44"/>
       <c r="B5" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="44"/>
       <c r="B6" s="16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="44"/>
       <c r="B7" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="44"/>
       <c r="B8" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="44"/>
       <c r="B9" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="45" t="s">
         <v>18</v>
       </c>
@@ -2143,19 +2165,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="45"/>
       <c r="B18" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="18"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>130</v>
       </c>
@@ -2179,14 +2201,14 @@
       <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2194,7 +2216,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -2203,7 +2225,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2212,7 +2234,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>55</v>
       </c>
@@ -2221,7 +2243,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -2230,7 +2252,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -2239,7 +2261,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>130</v>
       </c>
@@ -2248,7 +2270,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="50" t="s">
         <v>29</v>
       </c>
@@ -2263,7 +2285,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="51"/>
       <c r="B9" s="55"/>
       <c r="C9" s="59"/>
@@ -2272,7 +2294,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="51"/>
       <c r="B10" s="55"/>
       <c r="C10" s="59"/>
@@ -2281,7 +2303,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="51"/>
       <c r="B11" s="55"/>
       <c r="C11" s="59"/>
@@ -2290,7 +2312,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="51"/>
       <c r="B12" s="55"/>
       <c r="C12" s="59"/>
@@ -2299,7 +2321,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="51"/>
       <c r="B13" s="55"/>
       <c r="C13" s="59"/>
@@ -2308,7 +2330,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="51"/>
       <c r="B14" s="55"/>
       <c r="C14" s="60" t="s">
@@ -2319,7 +2341,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="51"/>
       <c r="B15" s="55"/>
       <c r="C15" s="60"/>
@@ -2328,7 +2350,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="51"/>
       <c r="B16" s="55"/>
       <c r="C16" s="60"/>
@@ -2337,7 +2359,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="51"/>
       <c r="B17" s="55"/>
       <c r="C17" s="60"/>
@@ -2346,7 +2368,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="51"/>
       <c r="B18" s="55"/>
       <c r="C18" s="61" t="s">
@@ -2357,7 +2379,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="51"/>
       <c r="B19" s="55"/>
       <c r="C19" s="61"/>
@@ -2366,7 +2388,7 @@
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="51"/>
       <c r="B20" s="55"/>
       <c r="C20" s="58" t="s">
@@ -2377,7 +2399,7 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="51"/>
       <c r="B21" s="55"/>
       <c r="C21" s="58"/>
@@ -2386,7 +2408,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="51"/>
       <c r="B22" s="55"/>
       <c r="C22" s="58"/>
@@ -2395,7 +2417,7 @@
       </c>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="51"/>
       <c r="B23" s="55"/>
       <c r="C23" s="58"/>
@@ -2404,7 +2426,7 @@
       </c>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="51"/>
       <c r="B24" s="55"/>
       <c r="C24" s="53" t="s">
@@ -2415,7 +2437,7 @@
       </c>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="51"/>
       <c r="B25" s="55"/>
       <c r="C25" s="53"/>
@@ -2424,7 +2446,7 @@
       </c>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="51"/>
       <c r="B26" s="55"/>
       <c r="C26" s="53"/>
@@ -2433,7 +2455,7 @@
       </c>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="51"/>
       <c r="B27" s="55"/>
       <c r="C27" s="53"/>
@@ -2442,7 +2464,7 @@
       </c>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="51"/>
       <c r="B28" s="55"/>
       <c r="C28" s="54" t="s">
@@ -2453,7 +2475,7 @@
       </c>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="51"/>
       <c r="B29" s="55"/>
       <c r="C29" s="54"/>
@@ -2462,7 +2484,7 @@
       </c>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="51"/>
       <c r="B30" s="55"/>
       <c r="C30" s="54"/>
@@ -2471,7 +2493,7 @@
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="51"/>
       <c r="B31" s="48" t="s">
         <v>51</v>
@@ -2482,7 +2504,7 @@
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="51"/>
       <c r="B32" s="48"/>
       <c r="C32" s="26" t="s">
@@ -2491,7 +2513,7 @@
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="51"/>
       <c r="B33" s="48"/>
       <c r="C33" s="26" t="s">
@@ -2500,7 +2522,7 @@
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="51"/>
       <c r="B34" s="48"/>
       <c r="C34" s="26" t="s">
@@ -2509,7 +2531,7 @@
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="51"/>
       <c r="B35" s="48"/>
       <c r="C35" s="47" t="s">
@@ -2520,7 +2542,7 @@
       </c>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="51"/>
       <c r="B36" s="48"/>
       <c r="C36" s="47"/>
@@ -2529,7 +2551,7 @@
       </c>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="51"/>
       <c r="B37" s="48"/>
       <c r="C37" s="47"/>
@@ -2540,7 +2562,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="51"/>
       <c r="B38" s="48"/>
       <c r="C38" s="47"/>
@@ -2549,7 +2571,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="51"/>
       <c r="B39" s="48"/>
       <c r="C39" s="47"/>
@@ -2558,7 +2580,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="51"/>
       <c r="B40" s="48"/>
       <c r="C40" s="47"/>
@@ -2567,7 +2589,7 @@
       </c>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="51"/>
       <c r="B41" s="48"/>
       <c r="C41" s="47"/>
@@ -2576,7 +2598,7 @@
       </c>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="51"/>
       <c r="B42" s="48"/>
       <c r="C42" s="47"/>
@@ -2585,7 +2607,7 @@
       </c>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="51"/>
       <c r="B43" s="48"/>
       <c r="C43" s="26" t="s">
@@ -2594,7 +2616,7 @@
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="51"/>
       <c r="B44" s="48"/>
       <c r="C44" s="26" t="s">
@@ -2603,7 +2625,7 @@
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="51"/>
       <c r="B45" s="48"/>
       <c r="C45" s="26" t="s">
@@ -2612,7 +2634,7 @@
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
     </row>
-    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="51"/>
       <c r="B46" s="48"/>
       <c r="C46" s="26" t="s">
@@ -2621,7 +2643,7 @@
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
     </row>
-    <row r="47" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="51"/>
       <c r="B47" s="56" t="s">
         <v>56</v>
@@ -2632,7 +2654,7 @@
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="51"/>
       <c r="B48" s="56"/>
       <c r="C48" s="20" t="s">
@@ -2641,7 +2663,7 @@
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="51"/>
       <c r="B49" s="49" t="s">
         <v>59</v>
@@ -2652,7 +2674,7 @@
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A50" s="51"/>
       <c r="B50" s="49"/>
       <c r="C50" s="29" t="s">
@@ -2661,7 +2683,7 @@
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A51" s="51"/>
       <c r="B51" s="49"/>
       <c r="C51" s="29" t="s">
@@ -2670,7 +2692,7 @@
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A52" s="51"/>
       <c r="B52" s="49"/>
       <c r="C52" s="29" t="s">
@@ -2679,7 +2701,7 @@
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
-    <row r="53" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A53" s="51"/>
       <c r="B53" s="49"/>
       <c r="C53" s="29" t="s">
@@ -2688,7 +2710,7 @@
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A54" s="51"/>
       <c r="B54" s="49"/>
       <c r="C54" s="29" t="s">
@@ -2697,7 +2719,7 @@
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A55" s="51"/>
       <c r="B55" s="49"/>
       <c r="C55" s="29" t="s">
@@ -2706,7 +2728,7 @@
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
     </row>
-    <row r="56" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A56" s="51"/>
       <c r="B56" s="49"/>
       <c r="C56" s="57" t="s">
@@ -2717,7 +2739,7 @@
       </c>
       <c r="E56" s="5"/>
     </row>
-    <row r="57" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A57" s="51"/>
       <c r="B57" s="49"/>
       <c r="C57" s="57"/>
@@ -2726,7 +2748,7 @@
       </c>
       <c r="E57" s="5"/>
     </row>
-    <row r="58" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A58" s="51"/>
       <c r="B58" s="49"/>
       <c r="C58" s="29" t="s">
@@ -2735,7 +2757,7 @@
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
     </row>
-    <row r="59" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A59" s="52"/>
       <c r="B59" s="19" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Modificación en la inserción de registro en la tabla de periodos y en la organización de las clases
</commit_message>
<xml_diff>
--- a/Recetatic/REcetario.xlsx
+++ b/Recetatic/REcetario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Script\source\repos\Recetatic\Recetatic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Worome\source\repos\Recetatic\Recetatic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4F9F6E-22BD-47BA-9AEA-347A889C2093}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAEBC0C-D079-4EBC-8F16-DA6591FD8814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="1" xr2:uid="{7CEDE6BF-7572-4931-BC0D-5229394BEFD2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{7CEDE6BF-7572-4931-BC0D-5229394BEFD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Funcionalidades" sheetId="2" r:id="rId1"/>
@@ -28,18 +28,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="165">
   <si>
     <t>EXPRESS</t>
   </si>
@@ -560,6 +554,24 @@
   </si>
   <si>
     <t>CharacterCasing</t>
+  </si>
+  <si>
+    <t>Hay que ver:</t>
+  </si>
+  <si>
+    <t>Mandar datos a Excel para imprimir</t>
+  </si>
+  <si>
+    <t>Mandar datos a Word para imprimir</t>
+  </si>
+  <si>
+    <t>Leer datos de una línea de un DataGridView</t>
+  </si>
+  <si>
+    <t>Tablas Maestro-Detalles</t>
+  </si>
+  <si>
+    <t>Ver instalación de Sql Server de distribución</t>
   </si>
 </sst>
 </file>
@@ -840,7 +852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -887,12 +899,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -965,10 +981,9 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1289,145 +1304,145 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.88671875" customWidth="1"/>
-    <col min="2" max="2" width="40.109375" customWidth="1"/>
+    <col min="1" max="1" width="45.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
         <v>80</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="38"/>
       <c r="B11" s="33" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
+    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="37" t="s">
         <v>151</v>
       </c>
       <c r="B17" s="31" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="37"/>
       <c r="B18" s="31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="37"/>
       <c r="B19" s="31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="36"/>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="37"/>
       <c r="B20" s="31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="37"/>
       <c r="B21" s="31" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="36"/>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="37"/>
       <c r="B22" s="31" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="36"/>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="37"/>
       <c r="B23" s="31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="37"/>
       <c r="B24" s="31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="36"/>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="37"/>
       <c r="B25" s="31" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="37"/>
       <c r="B26" s="31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>125</v>
       </c>
@@ -1444,133 +1459,166 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACFA3BB-9883-40C7-BCA9-F4350A092249}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>141</v>
       </c>
       <c r="B1" s="34" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="38"/>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="40"/>
       <c r="B2" s="34" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="40"/>
       <c r="B3" s="34" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
       <c r="B4" s="34" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="40"/>
       <c r="B5" s="34" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="38"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="40"/>
       <c r="B6" s="34" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="40"/>
       <c r="B7" s="34" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="40"/>
       <c r="B8" s="34" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="62" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="62"/>
-      <c r="B11" s="63" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="39"/>
+      <c r="B11" s="36" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="62"/>
-      <c r="B12" s="63" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="39"/>
+      <c r="B12" s="36" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="62"/>
-      <c r="B13" s="63" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="39"/>
+      <c r="B13" s="36" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="62"/>
-      <c r="B14" s="63" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="39"/>
+      <c r="B14" s="36" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="62"/>
-      <c r="B15" s="63" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="39"/>
+      <c r="B15" s="36" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
     </row>
-    <row r="21" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>154</v>
       </c>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="64" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="64"/>
+      <c r="B26" s="31" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="64"/>
+      <c r="B27" s="31" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="64"/>
+      <c r="B28" s="31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="64"/>
+      <c r="B29" s="31" t="s">
+        <v>164</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A10:A15"/>
     <mergeCell ref="A1:A8"/>
+    <mergeCell ref="A25:A29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1585,98 +1633,98 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
         <v>132</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="41"/>
       <c r="B4" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="41"/>
       <c r="B5" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="39"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="41"/>
       <c r="B6" s="11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>137</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>138</v>
       </c>
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>139</v>
       </c>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>127</v>
       </c>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>128</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>140</v>
       </c>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>60</v>
       </c>
@@ -1699,128 +1747,128 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>105</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>106</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="42" t="s">
         <v>107</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="42"/>
       <c r="B5" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="42"/>
       <c r="B6" s="12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>111</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>112</v>
       </c>
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>113</v>
       </c>
       <c r="B9" s="6"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>115</v>
       </c>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>116</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>117</v>
       </c>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>119</v>
       </c>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>120</v>
       </c>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>121</v>
       </c>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>122</v>
       </c>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>123</v>
       </c>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>124</v>
       </c>
@@ -1843,39 +1891,39 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>130</v>
       </c>
@@ -1894,35 +1942,35 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>99</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
         <v>100</v>
       </c>
       <c r="B4" s="14" t="s">
@@ -1930,45 +1978,45 @@
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="42"/>
-      <c r="B5" s="41" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="44"/>
+      <c r="B5" s="43" t="s">
         <v>102</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="42"/>
-      <c r="B6" s="41"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="44"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="42"/>
-      <c r="B7" s="41"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="44"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="42"/>
-      <c r="B8" s="41"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="44"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="13" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="42"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="44"/>
       <c r="B9" s="14" t="s">
         <v>103</v>
       </c>
       <c r="C9" s="14"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="42"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="44"/>
       <c r="B10" s="14" t="s">
         <v>11</v>
       </c>
@@ -1992,51 +2040,51 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>91</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="43" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
         <v>92</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="43"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="45"/>
       <c r="B5" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="43"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="45"/>
       <c r="B6" s="15" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="43"/>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
       <c r="B7" s="15" t="s">
         <v>96</v>
       </c>
@@ -2058,132 +2106,132 @@
       <selection activeCell="D1" sqref="D1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="46"/>
       <c r="B5" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="44"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="46"/>
       <c r="B6" s="16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="44"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="46"/>
       <c r="B7" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="44"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="46"/>
       <c r="B8" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="46"/>
       <c r="B9" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="6"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="6"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="6"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="45" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="47" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="45"/>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="47"/>
       <c r="B18" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="18"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>130</v>
       </c>
@@ -2207,14 +2255,14 @@
       <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2222,7 +2270,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -2231,7 +2279,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2240,7 +2288,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>55</v>
       </c>
@@ -2249,7 +2297,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -2258,7 +2306,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -2267,7 +2315,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>130</v>
       </c>
@@ -2276,14 +2324,14 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="50" t="s">
+    <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="61" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="20" t="s">
@@ -2291,55 +2339,55 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="51"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="59"/>
+    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="53"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="51"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="59"/>
+    <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="53"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="20" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="51"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="59"/>
+    <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="53"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="20" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="51"/>
-      <c r="B12" s="55"/>
-      <c r="C12" s="59"/>
+    <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="53"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="20" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="51"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="59"/>
+    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="53"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="20" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="51"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="60" t="s">
+    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="53"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="62" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="21" t="s">
@@ -2347,37 +2395,37 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="51"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="60"/>
+    <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="53"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="62"/>
       <c r="D15" s="21" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="51"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="60"/>
+    <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="53"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="62"/>
       <c r="D16" s="21" t="s">
         <v>34</v>
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="51"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="60"/>
+    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="53"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="62"/>
       <c r="D17" s="21" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="51"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="61" t="s">
+    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="53"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="63" t="s">
         <v>35</v>
       </c>
       <c r="D18" s="22" t="s">
@@ -2385,19 +2433,19 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="51"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="61"/>
+    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="53"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="63"/>
       <c r="D19" s="22" t="s">
         <v>37</v>
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="51"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="58" t="s">
+    <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="53"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="60" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="23" t="s">
@@ -2405,37 +2453,37 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A21" s="51"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="58"/>
+    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="53"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="60"/>
       <c r="D21" s="23" t="s">
         <v>40</v>
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A22" s="51"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="58"/>
+    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="53"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="60"/>
       <c r="D22" s="23" t="s">
         <v>41</v>
       </c>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="51"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="58"/>
+    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="53"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="60"/>
       <c r="D23" s="23" t="s">
         <v>42</v>
       </c>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A24" s="51"/>
-      <c r="B24" s="55"/>
-      <c r="C24" s="53" t="s">
+    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="53"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="55" t="s">
         <v>43</v>
       </c>
       <c r="D24" s="24" t="s">
@@ -2443,37 +2491,37 @@
       </c>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A25" s="51"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="53"/>
+    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="53"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="55"/>
       <c r="D25" s="24" t="s">
         <v>45</v>
       </c>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A26" s="51"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="53"/>
+    <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="53"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="55"/>
       <c r="D26" s="24" t="s">
         <v>46</v>
       </c>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A27" s="51"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="53"/>
+    <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="53"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="55"/>
       <c r="D27" s="24" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A28" s="51"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="54" t="s">
+    <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="53"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="56" t="s">
         <v>47</v>
       </c>
       <c r="D28" s="25" t="s">
@@ -2481,27 +2529,27 @@
       </c>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A29" s="51"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="54"/>
+    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="53"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="56"/>
       <c r="D29" s="25" t="s">
         <v>49</v>
       </c>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="51"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="54"/>
+    <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="53"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="56"/>
       <c r="D30" s="25" t="s">
         <v>50</v>
       </c>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A31" s="51"/>
-      <c r="B31" s="48" t="s">
+    <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="53"/>
+      <c r="B31" s="50" t="s">
         <v>51</v>
       </c>
       <c r="C31" s="26" t="s">
@@ -2510,37 +2558,37 @@
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A32" s="51"/>
-      <c r="B32" s="48"/>
+    <row r="32" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="53"/>
+      <c r="B32" s="50"/>
       <c r="C32" s="26" t="s">
         <v>52</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A33" s="51"/>
-      <c r="B33" s="48"/>
+    <row r="33" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="53"/>
+      <c r="B33" s="50"/>
       <c r="C33" s="26" t="s">
         <v>53</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
     </row>
-    <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A34" s="51"/>
-      <c r="B34" s="48"/>
+    <row r="34" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="53"/>
+      <c r="B34" s="50"/>
       <c r="C34" s="26" t="s">
         <v>54</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A35" s="51"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="47" t="s">
+    <row r="35" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="53"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="49" t="s">
         <v>66</v>
       </c>
       <c r="D35" s="27" t="s">
@@ -2548,110 +2596,110 @@
       </c>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A36" s="51"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="47"/>
+    <row r="36" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="53"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="49"/>
       <c r="D36" s="27" t="s">
         <v>68</v>
       </c>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="51"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="46" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="53"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="48" t="s">
         <v>69</v>
       </c>
       <c r="E37" s="28" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="51"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="46"/>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="53"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="51"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="47"/>
-      <c r="D39" s="46"/>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="53"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A40" s="51"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="47"/>
+    <row r="40" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="53"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="49"/>
       <c r="D40" s="27" t="s">
         <v>72</v>
       </c>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A41" s="51"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="47"/>
+    <row r="41" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="53"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="49"/>
       <c r="D41" s="27" t="s">
         <v>73</v>
       </c>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A42" s="51"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="47"/>
+    <row r="42" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="53"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="49"/>
       <c r="D42" s="27" t="s">
         <v>74</v>
       </c>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A43" s="51"/>
-      <c r="B43" s="48"/>
+    <row r="43" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="53"/>
+      <c r="B43" s="50"/>
       <c r="C43" s="26" t="s">
         <v>75</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A44" s="51"/>
-      <c r="B44" s="48"/>
+    <row r="44" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="53"/>
+      <c r="B44" s="50"/>
       <c r="C44" s="26" t="s">
         <v>76</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A45" s="51"/>
-      <c r="B45" s="48"/>
+    <row r="45" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="53"/>
+      <c r="B45" s="50"/>
       <c r="C45" s="26" t="s">
         <v>77</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
     </row>
-    <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A46" s="51"/>
-      <c r="B46" s="48"/>
+    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="53"/>
+      <c r="B46" s="50"/>
       <c r="C46" s="26" t="s">
         <v>78</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
     </row>
-    <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A47" s="51"/>
-      <c r="B47" s="56" t="s">
+    <row r="47" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="53"/>
+      <c r="B47" s="58" t="s">
         <v>56</v>
       </c>
       <c r="C47" s="20" t="s">
@@ -2660,18 +2708,18 @@
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A48" s="51"/>
-      <c r="B48" s="56"/>
+    <row r="48" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="53"/>
+      <c r="B48" s="58"/>
       <c r="C48" s="20" t="s">
         <v>58</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A49" s="51"/>
-      <c r="B49" s="49" t="s">
+    <row r="49" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="53"/>
+      <c r="B49" s="51" t="s">
         <v>59</v>
       </c>
       <c r="C49" s="29" t="s">
@@ -2680,64 +2728,64 @@
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A50" s="51"/>
-      <c r="B50" s="49"/>
+    <row r="50" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="53"/>
+      <c r="B50" s="51"/>
       <c r="C50" s="29" t="s">
         <v>60</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A51" s="51"/>
-      <c r="B51" s="49"/>
+    <row r="51" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="53"/>
+      <c r="B51" s="51"/>
       <c r="C51" s="29" t="s">
         <v>61</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A52" s="51"/>
-      <c r="B52" s="49"/>
+    <row r="52" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="53"/>
+      <c r="B52" s="51"/>
       <c r="C52" s="29" t="s">
         <v>16</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
-    <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A53" s="51"/>
-      <c r="B53" s="49"/>
+    <row r="53" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="53"/>
+      <c r="B53" s="51"/>
       <c r="C53" s="29" t="s">
         <v>62</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A54" s="51"/>
-      <c r="B54" s="49"/>
+    <row r="54" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="53"/>
+      <c r="B54" s="51"/>
       <c r="C54" s="29" t="s">
         <v>63</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A55" s="51"/>
-      <c r="B55" s="49"/>
+    <row r="55" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="53"/>
+      <c r="B55" s="51"/>
       <c r="C55" s="29" t="s">
         <v>17</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
     </row>
-    <row r="56" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A56" s="51"/>
-      <c r="B56" s="49"/>
-      <c r="C56" s="57" t="s">
+    <row r="56" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A56" s="53"/>
+      <c r="B56" s="51"/>
+      <c r="C56" s="59" t="s">
         <v>64</v>
       </c>
       <c r="D56" s="30" t="s">
@@ -2745,26 +2793,26 @@
       </c>
       <c r="E56" s="5"/>
     </row>
-    <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A57" s="51"/>
-      <c r="B57" s="49"/>
-      <c r="C57" s="57"/>
+    <row r="57" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="53"/>
+      <c r="B57" s="51"/>
+      <c r="C57" s="59"/>
       <c r="D57" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E57" s="5"/>
     </row>
-    <row r="58" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A58" s="51"/>
-      <c r="B58" s="49"/>
+    <row r="58" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="53"/>
+      <c r="B58" s="51"/>
       <c r="C58" s="29" t="s">
         <v>65</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
     </row>
-    <row r="59" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A59" s="52"/>
+    <row r="59" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="54"/>
       <c r="B59" s="19" t="s">
         <v>79</v>
       </c>

</xml_diff>